<commit_message>
fix(melee) : delete work sheet
</commit_message>
<xml_diff>
--- a/Datahandle/malee.xlsx
+++ b/Datahandle/malee.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -5057,28 +5055,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
chore(plot_grapg) : add excel file
</commit_message>
<xml_diff>
--- a/Datahandle/malee.xlsx
+++ b/Datahandle/malee.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="84" windowWidth="28740" windowHeight="12720"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="malee" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -493,9 +493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>